<commit_message>
new question and notification function
</commit_message>
<xml_diff>
--- a/data/reviews.xlsx
+++ b/data/reviews.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Имя баристы</t>
+          <t>Имя</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Фамилия</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
         </is>
       </c>
     </row>
@@ -478,6 +488,8 @@
           <t>Санжар</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -498,12 +510,12 @@
           <t>test</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2024-05-28</t>
-        </is>
+      <c r="A4" s="2" t="n">
+        <v>45440</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -519,6 +531,262 @@
         <is>
           <t>1</t>
         </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14:00:11.821246</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Sanzhar</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Karibay\</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>14:05:19.681022</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>14:28:39.047375</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Мухамедханов</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>14:29:56.165677</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>14:30:12.731676</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14:30:43.598356</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>14:32:49.106540</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sanzhar</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Karibay</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45441</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>14:34:13.195669</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Таха Хусейна 2/1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>507500572</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-05-29</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>19:35:54.122119</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Мухамедханов</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>sanzhar</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>karibay</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>507500572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add replacement function and fix time hh mm ss
</commit_message>
<xml_diff>
--- a/data/reviews.xlsx
+++ b/data/reviews.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karib\Desktop\work\TelegramBots\TelegramBots\DEVELOPING\lunacoffee_opening\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14891C78-CE0A-4FAD-886D-716538911218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118E23F7-3856-4D98-B218-5A375C43DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Дата</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Точка</t>
+  </si>
+  <si>
+    <t>Статус</t>
   </si>
   <si>
     <t>Имя</t>
@@ -400,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,6 +429,9 @@
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>